<commit_message>
added median salary bar graphs
</commit_message>
<xml_diff>
--- a/Median salary for doctoral recipients.xlsx
+++ b/Median salary for doctoral recipients.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D97E34-526E-AA44-A470-965A9FB746B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF229B1-F5BC-0046-AA55-CF993CFB039A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="28800" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,19 +113,23 @@
       <b/>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -650,7 +654,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:C20"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>